<commit_message>
Segmentador de datos en tablas
</commit_message>
<xml_diff>
--- a/Excel/Sección 2/Ventas.xlsx
+++ b/Excel/Sección 2/Ventas.xlsx
@@ -15,8 +15,23 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
     <sheet name="Copia" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="SegmentaciónDeDatos_Producto">#N/A</definedName>
+    <definedName name="SegmentaciónDeDatos_Region">#N/A</definedName>
+    <definedName name="SegmentaciónDeDatos_Vendedor">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
+      <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicerCache r:id="rId3"/>
+        <x14:slicerCache r:id="rId4"/>
+        <x14:slicerCache r:id="rId5"/>
+      </x15:slicerCaches>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="17">
   <si>
     <t>Region</t>
   </si>
@@ -73,6 +88,9 @@
   </si>
   <si>
     <t>Sara</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -81,7 +99,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -115,34 +133,14 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="1">
     <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -157,8 +155,267 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38325</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>117000</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Region"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Region"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3819750" y="0"/>
+              <a:ext cx="1800000" cy="1260000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-AR" sz="1100"/>
+                <a:t>Esta forma representa una segmentación de datos de tabla. La segmentación de datos de tabla se admite en Excel 2013 o versiones posteriores.
+Si la forma se modificó en una versión anterior de Excel o si el libro se guardó en Excel 2007 o una versión anterior, no se puede usar la segmentación de datos.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>126525</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Vendedor"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Vendedor"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3810225" y="1533525"/>
+              <a:ext cx="1800000" cy="1260000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-AR" sz="1100"/>
+                <a:t>Esta forma representa una segmentación de datos de tabla. La segmentación de datos de tabla se admite en Excel 2013 o versiones posteriores.
+Si la forma se modificó en una versión anterior de Excel o si el libro se guardó en Excel 2007 o una versión anterior, no se puede usar la segmentación de datos.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>117000</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Producto"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Producto"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3810225" y="3048000"/>
+              <a:ext cx="1800000" cy="1260000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-AR" sz="1100"/>
+                <a:t>Esta forma representa una segmentación de datos de tabla. La segmentación de datos de tabla se admite en Excel 2013 o versiones posteriores.
+Si la forma se modificó en una versión anterior de Excel o si el libro se guardó en Excel 2007 o una versión anterior, no se puede usar la segmentación de datos.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Region" sourceName="Region">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="1" column="1"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Vendedor" sourceName="Vendedor">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="1" column="3"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Producto" sourceName="Producto">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="1" column="2"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Region" cache="SegmentaciónDeDatos_Region" caption="Region" rowHeight="241300"/>
+  <slicer name="Vendedor" cache="SegmentaciónDeDatos_Vendedor" caption="Vendedor" columnCount="2" style="SlicerStyleLight4" rowHeight="241300"/>
+  <slicer name="Producto" cache="SegmentaciónDeDatos_Producto" caption="Producto" style="SlicerStyleLight6" rowHeight="241300"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaVentas" displayName="TablaVentas" ref="A1:D19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaVentas" displayName="TablaVentas" ref="A1:D20" totalsRowCount="1">
   <autoFilter ref="A1:D19"/>
   <sortState ref="A2:D19">
     <sortCondition ref="C1:C19"/>
@@ -167,7 +424,7 @@
     <tableColumn id="1" name="Region" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Producto"/>
     <tableColumn id="3" name="Vendedor"/>
-    <tableColumn id="4" name="Ventas" totalsRowFunction="sum" dataDxfId="2"/>
+    <tableColumn id="4" name="Ventas" totalsRowFunction="sum" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="1" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -436,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,6 +970,15 @@
       </c>
       <c r="D19" s="2">
         <v>23151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="2">
+        <f>SUBTOTAL(109,TablaVentas[Ventas])</f>
+        <v>239533</v>
       </c>
     </row>
   </sheetData>
@@ -728,9 +994,17 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
+      <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicer r:id="rId4"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Tabla dinamica y filtro de datos
</commit_message>
<xml_diff>
--- a/Excel/Sección 2/Ventas.xlsx
+++ b/Excel/Sección 2/Ventas.xlsx
@@ -9,27 +9,37 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="14925"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="14925" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Copia" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja4" sheetId="6" r:id="rId1"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Copia" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="SegmentaciónDeDatos_Producto">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_Region">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_Vendedor">#N/A</definedName>
+    <definedName name="SegmentaciónDeDatos_Vendedor1">#N/A</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <pivotCaches>
+    <pivotCache cacheId="16" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId5"/>
+      </x14:slicerCaches>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId3"/>
-        <x14:slicerCache r:id="rId4"/>
-        <x14:slicerCache r:id="rId5"/>
+        <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
+        <x14:slicerCache r:id="rId8"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="19">
   <si>
     <t>Region</t>
   </si>
@@ -90,14 +100,21 @@
     <t>Sara</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Suma de Ventas</t>
+  </si>
+  <si>
+    <t>Total general</t>
+  </si>
+  <si>
+    <t>(Todas)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -130,15 +147,230 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="70">
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -170,8 +402,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>117000</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Region"/>
@@ -188,7 +420,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -242,8 +474,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>126525</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Vendedor"/>
@@ -260,7 +492,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -314,8 +546,8 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>117000</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Producto"/>
@@ -332,7 +564,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -373,10 +605,361 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Vendedor 1"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Vendedor 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9477375" y="190500"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-AR" sz="1100"/>
+                <a:t>Esta forma representa una segmentación de datos. La segmentación de datos se admite en Excel 2010 y versiones posteriores.
+Si la forma se modificó en una versión anterior de Excel o si el libro se guardó en Excel 2003 o una versión anterior, no se puede usar la segmentación de datos.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Braian" refreshedDate="44951.79046261574" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="18">
+  <cacheSource type="worksheet">
+    <worksheetSource name="TablaVentas"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Este"/>
+        <s v="Central"/>
+        <s v="Oeste"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Producto" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Accesorios"/>
+        <s v="Dispositivos"/>
+        <s v="Sistemas"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Vendedor" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Ana"/>
+        <s v="David"/>
+        <s v="Karen"/>
+        <s v="Kevin"/>
+        <s v="Lucas"/>
+        <s v="Sara"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Ventas" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4744" maxValue="32855"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="18">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9323"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="10348"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="13531"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="8287"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="11420"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="20098"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="6909"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="12948"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="30633"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4744"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="10711"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="32855"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="7667"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="9312"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="13374"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="5442"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="8780"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="23151"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica6" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Region">
+  <location ref="J3:K16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Suma de Ventas" fld="3" baseField="0" baseItem="0" numFmtId="41"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="30">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium6" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Vendedor1" sourceName="Vendedor">
+  <pivotTables>
+    <pivotTable tabId="1" name="Tabla dinámica6"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1">
+      <items count="6">
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="4" s="1"/>
+        <i x="5" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Region" sourceName="Region">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
@@ -386,7 +969,7 @@
 </slicerCacheDefinition>
 </file>
 
-<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Vendedor" sourceName="Vendedor">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
@@ -396,7 +979,7 @@
 </slicerCacheDefinition>
 </file>
 
-<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Producto" sourceName="Producto">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
@@ -408,6 +991,12 @@
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Vendedor 1" cache="SegmentaciónDeDatos_Vendedor1" caption="Vendedor" rowHeight="241300"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="Region" cache="SegmentaciónDeDatos_Region" caption="Region" rowHeight="241300"/>
   <slicer name="Vendedor" cache="SegmentaciónDeDatos_Vendedor" caption="Vendedor" columnCount="2" style="SlicerStyleLight4" rowHeight="241300"/>
   <slicer name="Producto" cache="SegmentaciónDeDatos_Producto" caption="Producto" style="SlicerStyleLight6" rowHeight="241300"/>
@@ -415,7 +1004,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaVentas" displayName="TablaVentas" ref="A1:D20" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Region"/>
+    <tableColumn id="2" name="Producto"/>
+    <tableColumn id="3" name="Vendedor"/>
+    <tableColumn id="4" name="Ventas"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaVentas" displayName="TablaVentas" ref="A1:D19">
   <autoFilter ref="A1:D19"/>
   <sortState ref="A2:D19">
     <sortCondition ref="C1:C19"/>
@@ -424,7 +1026,7 @@
     <tableColumn id="1" name="Region" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Producto"/>
     <tableColumn id="3" name="Vendedor"/>
-    <tableColumn id="4" name="Ventas" totalsRowFunction="sum" dataDxfId="0"/>
+    <tableColumn id="4" name="Ventas" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="1" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -693,10 +1295,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>6909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>8287</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,9 +1369,14 @@
     <col min="1" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,8 +1389,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -733,8 +1409,9 @@
       <c r="D2" s="2">
         <v>9323</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -747,8 +1424,14 @@
       <c r="D3" s="2">
         <v>10348</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -761,8 +1444,14 @@
       <c r="D4" s="2">
         <v>13531</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="6">
+        <v>90295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -775,8 +1464,14 @@
       <c r="D5" s="2">
         <v>8287</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="6">
+        <v>15196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -789,8 +1484,14 @@
       <c r="D6" s="2">
         <v>11420</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="6">
+        <v>24368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -803,8 +1504,14 @@
       <c r="D7" s="2">
         <v>20098</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="6">
+        <v>50731</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -817,8 +1524,14 @@
       <c r="D8" s="2">
         <v>6909</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="6">
+        <v>63555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -831,8 +1544,14 @@
       <c r="D9" s="2">
         <v>12948</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="6">
+        <v>16990</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -845,8 +1564,14 @@
       <c r="D10" s="2">
         <v>30633</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="6">
+        <v>19660</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -859,8 +1584,14 @@
       <c r="D11" s="2">
         <v>4744</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="6">
+        <v>26905</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -873,8 +1604,14 @@
       <c r="D12" s="2">
         <v>10711</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="6">
+        <v>85683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -887,8 +1624,14 @@
       <c r="D13" s="2">
         <v>32855</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="6">
+        <v>10186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -901,8 +1644,14 @@
       <c r="D14" s="2">
         <v>7667</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="6">
+        <v>19491</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -915,8 +1664,14 @@
       <c r="D15" s="2">
         <v>9312</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="6">
+        <v>56006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -929,8 +1684,14 @@
       <c r="D16" s="2">
         <v>13374</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="6">
+        <v>239533</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -943,8 +1704,9 @@
       <c r="D17" s="2">
         <v>5442</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -957,8 +1719,9 @@
       <c r="D18" s="2">
         <v>8780</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -970,15 +1733,6 @@
       </c>
       <c r="D19" s="2">
         <v>23151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="2">
-        <f>SUBTOTAL(109,TablaVentas[Ventas])</f>
-        <v>239533</v>
       </c>
     </row>
   </sheetData>
@@ -993,22 +1747,27 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId5"/>
+      </x14:slicerList>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId4"/>
+        <x14:slicer r:id="rId6"/>
       </x14:slicerList>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Graficos recomendados de tablas
</commit_message>
<xml_diff>
--- a/Excel/Sección 2/Ventas.xlsx
+++ b/Excel/Sección 2/Ventas.xlsx
@@ -12,9 +12,8 @@
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="14925" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja4" sheetId="6" r:id="rId1"/>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId2"/>
-    <sheet name="Copia" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Copia" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="SegmentaciónDeDatos_Producto">#N/A</definedName>
@@ -24,12 +23,12 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId5"/>
+        <x14:slicerCache r:id="rId4"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -37,9 +36,9 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicerCache r:id="rId5"/>
         <x14:slicerCache r:id="rId6"/>
         <x14:slicerCache r:id="rId7"/>
-        <x14:slicerCache r:id="rId8"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="19">
   <si>
     <t>Region</t>
   </si>
@@ -106,7 +105,7 @@
     <t>Total general</t>
   </si>
   <si>
-    <t>(Todas)</t>
+    <t>Etiquetas de columna</t>
   </si>
 </sst>
 </file>
@@ -147,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -159,13 +158,19 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -179,201 +184,6 @@
     <dxf>
       <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="32" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -385,6 +195,3277 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Ventas.xlsx]Hoja 1!TD-Ventas</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hoja 1'!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Hoja 1'!$J$4:$J$34</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="18"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>David</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Karen</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>David</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Karen</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>David</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Karen</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Ana</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Lucas</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Ana</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Lucas</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Ana</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Lucas</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Kevin</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Sara</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Kevin</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Sara</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Kevin</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Sara</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Central</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Este</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Oeste</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$K$4:$K$34</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>8287</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11420</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20098</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30633</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9323</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10348</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9312</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13531</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13374</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4744</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5442</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10711</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8780</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32855</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="314719336"/>
+        <c:axId val="314723648"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="314719336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="314723648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="314723648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="314719336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Ventas.xlsx]Hoja 1!TB-Ventas2</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hoja 1'!$N$3:$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ana</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Hoja 1'!$M$5:$M$17</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Central</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Este</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Oeste</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$N$5:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="3">
+                  <c:v>9323</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10348</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hoja 1'!$O$3:$O$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>David</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Hoja 1'!$M$5:$M$17</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Central</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Este</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Oeste</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$O$5:$O$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8287</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11420</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hoja 1'!$P$3:$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Karen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Hoja 1'!$M$5:$M$17</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Central</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Este</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Oeste</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$P$5:$P$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12948</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30633</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hoja 1'!$Q$3:$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kevin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Hoja 1'!$M$5:$M$17</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Central</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Este</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Oeste</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$Q$5:$Q$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="6">
+                  <c:v>4744</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10711</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32855</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hoja 1'!$R$3:$R$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lucas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Hoja 1'!$M$5:$M$17</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Central</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Este</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Oeste</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$R$5:$R$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="3">
+                  <c:v>7667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13374</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hoja 1'!$S$3:$S$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sara</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Hoja 1'!$M$5:$M$17</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Accesorios</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Dispositivos</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sistemas</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Central</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Este</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Oeste</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$S$5:$S$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="6">
+                  <c:v>5442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8780</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="368861528"/>
+        <c:axId val="368861136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="368861528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="368861136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="368861136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="368861528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -607,19 +3688,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>441157</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>170447</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>715376</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>27572</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Vendedor 1"/>
@@ -636,7 +3717,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -646,8 +3727,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9477375" y="190500"/>
-              <a:ext cx="1828800" cy="2524125"/>
+              <a:off x="1195220" y="3940760"/>
+              <a:ext cx="1831953" cy="2496343"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -675,6 +3756,66 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1092398</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47228</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>296664</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>151210</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>298648</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>156369</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>167679</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71835</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -836,8 +3977,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica6" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Region">
-  <location ref="J3:K16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TB-Ventas2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Region">
+  <location ref="M3:S17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -855,7 +3996,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisPage" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="7">
         <item x="0"/>
         <item x="1"/>
@@ -913,24 +4054,282 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
   </colItems>
-  <pageFields count="1">
-    <pageField fld="2" hier="-1"/>
-  </pageFields>
   <dataFields count="1">
     <dataField name="Suma de Ventas" fld="3" baseField="0" baseItem="0" numFmtId="41"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="30">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium6" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleDark9" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="1" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TD-Ventas" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Region">
+  <location ref="J3:K34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="31">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Ventas" fld="3" baseField="0" baseItem="0" numFmtId="41"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="5">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleMedium6" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="1" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -942,7 +4341,7 @@
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaciónDeDatos_Vendedor1" sourceName="Vendedor">
   <pivotTables>
-    <pivotTable tabId="1" name="Tabla dinámica6"/>
+    <pivotTable tabId="1" name="TD-Ventas"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
@@ -1004,19 +4403,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A1:D3" totalsRowShown="0">
-  <autoFilter ref="A1:D3"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Region"/>
-    <tableColumn id="2" name="Producto"/>
-    <tableColumn id="3" name="Vendedor"/>
-    <tableColumn id="4" name="Ventas"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaVentas" displayName="TablaVentas" ref="A1:D19">
   <autoFilter ref="A1:D19"/>
   <sortState ref="A2:D19">
@@ -1026,7 +4412,7 @@
     <tableColumn id="1" name="Region" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Producto"/>
     <tableColumn id="3" name="Vendedor"/>
-    <tableColumn id="4" name="Ventas" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="4" name="Ventas" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="1" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1295,73 +4681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>6909</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>8287</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="L9" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,12 +4694,14 @@
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1389,14 +4714,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
+      <c r="K1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +4731,7 @@
       </c>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1430,8 +4750,14 @@
       <c r="K3" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="M3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1450,8 +4776,29 @@
       <c r="K4" s="6">
         <v>90295</v>
       </c>
+      <c r="M4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1470,8 +4817,21 @@
       <c r="K5" s="6">
         <v>15196</v>
       </c>
+      <c r="M5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6">
+        <v>39805</v>
+      </c>
+      <c r="P5" s="6">
+        <v>50490</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1484,14 +4844,27 @@
       <c r="D6" s="2">
         <v>11420</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>8</v>
+      <c r="J6" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="K6" s="6">
-        <v>24368</v>
-      </c>
+        <v>8287</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6">
+        <v>8287</v>
+      </c>
+      <c r="P6" s="6">
+        <v>6909</v>
+      </c>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1504,14 +4877,27 @@
       <c r="D7" s="2">
         <v>20098</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>9</v>
+      <c r="J7" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="K7" s="6">
-        <v>50731</v>
-      </c>
+        <v>6909</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6">
+        <v>11420</v>
+      </c>
+      <c r="P7" s="6">
+        <v>12948</v>
+      </c>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1524,14 +4910,27 @@
       <c r="D8" s="2">
         <v>6909</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>10</v>
+      <c r="J8" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="K8" s="6">
-        <v>63555</v>
-      </c>
+        <v>24368</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6">
+        <v>20098</v>
+      </c>
+      <c r="P8" s="6">
+        <v>30633</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1544,14 +4943,27 @@
       <c r="D9" s="2">
         <v>12948</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>5</v>
+      <c r="J9" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="K9" s="6">
-        <v>16990</v>
-      </c>
+        <v>11420</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="6">
+        <v>33202</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6">
+        <v>30353</v>
+      </c>
+      <c r="S9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1564,14 +4976,27 @@
       <c r="D10" s="2">
         <v>30633</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>8</v>
+      <c r="J10" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="K10" s="6">
-        <v>19660</v>
-      </c>
+        <v>12948</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="6">
+        <v>9323</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6">
+        <v>7667</v>
+      </c>
+      <c r="S10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1588,10 +5013,23 @@
         <v>9</v>
       </c>
       <c r="K11" s="6">
-        <v>26905</v>
-      </c>
+        <v>50731</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="6">
+        <v>10348</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6">
+        <v>9312</v>
+      </c>
+      <c r="S11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1604,14 +5042,27 @@
       <c r="D12" s="2">
         <v>10711</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>13</v>
+      <c r="J12" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="K12" s="6">
-        <v>85683</v>
-      </c>
+        <v>20098</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="6">
+        <v>13531</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6">
+        <v>13374</v>
+      </c>
+      <c r="S12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1624,14 +5075,27 @@
       <c r="D13" s="2">
         <v>32855</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>5</v>
+      <c r="J13" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="K13" s="6">
-        <v>10186</v>
+        <v>30633</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6">
+        <v>48310</v>
+      </c>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6">
+        <v>37373</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1644,14 +5108,27 @@
       <c r="D14" s="2">
         <v>7667</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>8</v>
+      <c r="J14" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="K14" s="6">
-        <v>19491</v>
+        <v>63555</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6">
+        <v>4744</v>
+      </c>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6">
+        <v>5442</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1665,13 +5142,26 @@
         <v>9312</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K15" s="6">
-        <v>56006</v>
+        <v>16990</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6">
+        <v>10711</v>
+      </c>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6">
+        <v>8780</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1684,14 +5174,27 @@
       <c r="D16" s="2">
         <v>13374</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>17</v>
+      <c r="J16" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="K16" s="6">
-        <v>239533</v>
+        <v>9323</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6">
+        <v>32855</v>
+      </c>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6">
+        <v>23151</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1704,9 +5207,35 @@
       <c r="D17" s="2">
         <v>5442</v>
       </c>
-      <c r="K17"/>
+      <c r="J17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="6">
+        <v>7667</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="6">
+        <v>33202</v>
+      </c>
+      <c r="O17" s="6">
+        <v>39805</v>
+      </c>
+      <c r="P17" s="6">
+        <v>50490</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>48310</v>
+      </c>
+      <c r="R17" s="6">
+        <v>30353</v>
+      </c>
+      <c r="S17" s="6">
+        <v>37373</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1719,9 +5248,14 @@
       <c r="D18" s="2">
         <v>8780</v>
       </c>
-      <c r="K18"/>
+      <c r="J18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="6">
+        <v>19660</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1733,6 +5267,132 @@
       </c>
       <c r="D19" s="2">
         <v>23151</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="6">
+        <v>10348</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="6">
+        <v>9312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="6">
+        <v>26905</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="6">
+        <v>13531</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="6">
+        <v>13374</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="6">
+        <v>85683</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K25" s="6">
+        <v>10186</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26" s="6">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="6">
+        <v>5442</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="6">
+        <v>19491</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K29" s="6">
+        <v>10711</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="6">
+        <v>8780</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="6">
+        <v>56006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="6">
+        <v>32855</v>
+      </c>
+    </row>
+    <row r="33" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="6">
+        <v>23151</v>
+      </c>
+    </row>
+    <row r="34" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K34" s="6">
+        <v>239533</v>
       </c>
     </row>
   </sheetData>
@@ -1747,32 +5407,32 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
       <x14:slicerList>
-        <x14:slicer r:id="rId5"/>
+        <x14:slicer r:id="rId6"/>
       </x14:slicerList>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId6"/>
+        <x14:slicer r:id="rId7"/>
       </x14:slicerList>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>